<commit_message>
p3ht literature transfer to template
attempt 2, small subset of data from paper
</commit_message>
<xml_diff>
--- a/db_feed/P3HT/Literature/Literature_1/L1.xlsx
+++ b/db_feed/P3HT/Literature/Literature_1/L1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\volko\Desktop\Grover\DB\ofet-db\db_feed\P3HT\Literature\Literature_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E439D0-2492-4248-BF7D-CC58A68630B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8BBDCCB3-2248-4E9C-B281-69038E966310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F8B411A1-6901-4B9B-966C-09D3D94CB0BB}"/>
+    <workbookView xWindow="9990" yWindow="-9495" windowWidth="17280" windowHeight="8880" firstSheet="2" activeTab="3" xr2:uid="{F8B411A1-6901-4B9B-966C-09D3D94CB0BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Legend" sheetId="7" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="393">
   <si>
     <t>Solution Information</t>
   </si>
@@ -1325,6 +1325,30 @@
     <t>Film - (100) coherence length</t>
   </si>
   <si>
+    <t>Measurement Type</t>
+  </si>
+  <si>
+    <t>Semiconductor Parameter Analyzer</t>
+  </si>
+  <si>
+    <t>Time of Flight</t>
+  </si>
+  <si>
+    <t>Conductivity</t>
+  </si>
+  <si>
+    <t>Transfer Curve - mobility regime</t>
+  </si>
+  <si>
+    <t>Measurement Regime</t>
+  </si>
+  <si>
+    <t>saturation</t>
+  </si>
+  <si>
+    <t>linear</t>
+  </si>
+  <si>
     <t>Ron</t>
   </si>
   <si>
@@ -1334,61 +1358,16 @@
     <t>rvolkovinsky3@gatech.edu</t>
   </si>
   <si>
-    <t>publications</t>
+    <t>experiments</t>
   </si>
   <si>
-    <t>experiments</t>
+    <t>publications</t>
   </si>
   <si>
     <t>10.1002/adfm.201002729</t>
   </si>
   <si>
-    <t>Wiley</t>
-  </si>
-  <si>
-    <t>Advanced Functional Materials</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tunable Crystallinity in Regioregular Poly(3-Hexylthiophene) Thin Films and Its Impact on Field Effect Mobility </t>
-  </si>
-  <si>
-    <t>Author #3</t>
-  </si>
-  <si>
-    <t>Author #4</t>
-  </si>
-  <si>
-    <t>Author #5</t>
-  </si>
-  <si>
-    <t>Avishek R. Aiyar</t>
-  </si>
-  <si>
-    <t>Jung-Il Hong</t>
-  </si>
-  <si>
-    <t>Rakesh Nambiar</t>
-  </si>
-  <si>
-    <t>David M. Collard</t>
-  </si>
-  <si>
-    <t>Elsa Reichmanis</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1002/adfm.201002729</t>
-  </si>
-  <si>
-    <t>English</t>
-  </si>
-  <si>
-    <t>Georgia Institute of Technology</t>
-  </si>
-  <si>
-    <t>CHCl3</t>
-  </si>
-  <si>
-    <t>Sigma Aldrich</t>
+    <t>Sigma Aldritch</t>
   </si>
   <si>
     <t>Bransonic 2510</t>
@@ -1397,16 +1376,16 @@
     <t>Sealed glass vial</t>
   </si>
   <si>
-    <t>Agilent 4155C semiconductor parameter analyzer</t>
+    <t>Agilent 4155C</t>
   </si>
   <si>
     <t>Agilent 8510</t>
   </si>
   <si>
-    <t>Panalytical X'Pert Pro</t>
+    <t>Veeco Digital Instruments Dimension 3100</t>
   </si>
   <si>
-    <t>Veeco Digital Instruments Dimension 3100</t>
+    <t>Panalytical X'pert Pro</t>
   </si>
 </sst>
 </file>
@@ -2186,7 +2165,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2346,10 +2325,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2688,8 +2663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE1795BC-75E9-4640-AF6F-D5B4268C1FF0}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
@@ -2730,8 +2705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A5882D5-D74D-473F-B8FF-8824B9621A3C}">
   <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="114" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView topLeftCell="A28" zoomScale="114" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
@@ -3231,7 +3206,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:4">
       <c r="A49" t="s">
         <v>361</v>
       </c>
@@ -3239,46 +3214,67 @@
         <v>161</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:4">
       <c r="A50" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:4">
       <c r="A52" s="2" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:4">
       <c r="A53" s="23" t="s">
         <v>97</v>
       </c>
       <c r="B53" s="23" t="s">
         <v>94</v>
       </c>
+      <c r="C53" t="s">
+        <v>372</v>
+      </c>
+      <c r="D53" t="s">
+        <v>377</v>
+      </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:4">
       <c r="A55" t="s">
         <v>159</v>
       </c>
       <c r="B55" t="s">
         <v>163</v>
       </c>
+      <c r="C55" t="s">
+        <v>373</v>
+      </c>
+      <c r="D55" t="s">
+        <v>378</v>
+      </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:4">
       <c r="A56" t="s">
         <v>160</v>
       </c>
       <c r="B56" t="s">
         <v>164</v>
       </c>
+      <c r="C56" t="s">
+        <v>374</v>
+      </c>
+      <c r="D56" t="s">
+        <v>379</v>
+      </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:4">
       <c r="A57" t="s">
         <v>161</v>
       </c>
       <c r="B57" t="s">
         <v>364</v>
+      </c>
+      <c r="C57" t="s">
+        <v>375</v>
       </c>
     </row>
   </sheetData>
@@ -3289,10 +3285,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87527978-2A5B-6545-88F5-0DA220A53CEB}">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
@@ -3314,10 +3310,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.6">
-      <c r="A2" s="109" t="s">
+      <c r="A2" s="107" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="109"/>
+      <c r="B2" s="107"/>
       <c r="C2" s="8"/>
     </row>
     <row r="3" spans="1:3" ht="15.6">
@@ -3325,7 +3321,7 @@
         <v>165</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>372</v>
+        <v>380</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>61</v>
@@ -3336,7 +3332,7 @@
         <v>166</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>373</v>
+        <v>381</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.6">
@@ -3344,7 +3340,7 @@
         <v>62</v>
       </c>
       <c r="B5" s="33" t="s">
-        <v>374</v>
+        <v>382</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.6">
@@ -3352,7 +3348,7 @@
         <v>63</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>376</v>
+        <v>383</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.6">
@@ -3360,7 +3356,7 @@
         <v>64</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>375</v>
+        <v>384</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.6">
@@ -3381,7 +3377,7 @@
         <v>66</v>
       </c>
       <c r="B10" s="34" t="s">
-        <v>377</v>
+        <v>385</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>169</v>
@@ -3406,33 +3402,25 @@
       <c r="A15" t="s">
         <v>167</v>
       </c>
-      <c r="B15" s="32" t="s">
-        <v>378</v>
-      </c>
+      <c r="B15" s="32"/>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>168</v>
       </c>
-      <c r="B16" s="32" t="s">
-        <v>379</v>
-      </c>
+      <c r="B16" s="32"/>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>68</v>
       </c>
-      <c r="B17" s="32" t="s">
-        <v>380</v>
-      </c>
+      <c r="B17" s="32"/>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>69</v>
       </c>
-      <c r="B18" s="32" t="s">
-        <v>384</v>
-      </c>
+      <c r="B18" s="32"/>
       <c r="C18" s="10" t="s">
         <v>70</v>
       </c>
@@ -3441,146 +3429,106 @@
       <c r="A19" t="s">
         <v>71</v>
       </c>
-      <c r="B19" s="32" t="s">
-        <v>385</v>
-      </c>
+      <c r="B19" s="32"/>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>381</v>
+        <v>72</v>
       </c>
-      <c r="B20" s="32" t="s">
-        <v>386</v>
-      </c>
+      <c r="B20" s="32"/>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>382</v>
+        <v>73</v>
       </c>
-      <c r="B21" s="32" t="s">
-        <v>387</v>
-      </c>
+      <c r="B21" s="32"/>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>383</v>
+        <v>74</v>
       </c>
-      <c r="B22" s="32" t="s">
-        <v>388</v>
-      </c>
+      <c r="B22" s="32"/>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B23" s="32"/>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B24" s="32"/>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
-      <c r="B25" s="32">
-        <v>2011</v>
-      </c>
+      <c r="B25" s="32"/>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
-      <c r="B26" s="32">
-        <v>21</v>
-      </c>
+      <c r="B26" s="32"/>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
-      <c r="B27" s="32">
-        <v>14</v>
+      <c r="B27" s="32"/>
+      <c r="C27" s="4" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
-      <c r="B28" s="107" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" t="s">
-        <v>78</v>
-      </c>
-      <c r="B29" s="32" t="s">
-        <v>390</v>
+      <c r="B28" s="35"/>
+      <c r="C28" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" t="s">
-        <v>79</v>
+      <c r="A30" s="13" t="s">
+        <v>83</v>
       </c>
-      <c r="B30" s="32" t="s">
-        <v>391</v>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+    </row>
+    <row r="31" spans="1:3" ht="15.6">
+      <c r="A31" s="9" t="s">
+        <v>84</v>
       </c>
-      <c r="C30" s="4" t="s">
-        <v>80</v>
+      <c r="B31"/>
+      <c r="C31"/>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>85</v>
       </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" t="s">
-        <v>81</v>
-      </c>
-      <c r="B31" s="35">
-        <v>44859</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="B32" s="35"/>
+      <c r="C32" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="13" t="s">
-        <v>83</v>
+      <c r="A33" t="s">
+        <v>86</v>
       </c>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-    </row>
-    <row r="34" spans="1:3" ht="15.6">
-      <c r="A34" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="B34"/>
-      <c r="C34"/>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" t="s">
-        <v>85</v>
-      </c>
-      <c r="B35" s="35"/>
-      <c r="C35" t="s">
+      <c r="B33" s="35"/>
+      <c r="C33" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
-      <c r="A36" t="s">
-        <v>86</v>
-      </c>
-      <c r="B36" s="35"/>
-      <c r="C36" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="4" t="s">
+    <row r="34" spans="1:3">
+      <c r="A34" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B37" s="35"/>
-      <c r="C37" s="4" t="s">
+      <c r="B34" s="35"/>
+      <c r="C34" s="4" t="s">
         <v>232</v>
       </c>
     </row>
@@ -3637,11 +3585,10 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" xr:uid="{633C8518-24A4-48E6-A977-FDEAE75576F8}"/>
-    <hyperlink ref="B28" r:id="rId2" xr:uid="{4A2F8AF1-4C46-4CAA-A77B-5656DE114D9A}"/>
+    <hyperlink ref="B5" r:id="rId1" xr:uid="{4B0EABAF-3771-4B0A-A14C-899F6C700598}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
@@ -3674,7 +3621,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
@@ -3721,8 +3668,8 @@
       <c r="A5" s="91" t="s">
         <v>183</v>
       </c>
-      <c r="B5" s="90" t="s">
-        <v>392</v>
+      <c r="B5" s="97" t="s">
+        <v>180</v>
       </c>
       <c r="C5" s="83"/>
       <c r="D5" s="83" t="s">
@@ -3736,7 +3683,7 @@
       <c r="A6" s="92" t="s">
         <v>8</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="90">
         <v>100</v>
       </c>
       <c r="C6" t="s">
@@ -3785,7 +3732,7 @@
       <c r="A10" s="92" t="s">
         <v>177</v>
       </c>
-      <c r="B10" s="108" t="s">
+      <c r="B10" s="89" t="s">
         <v>119</v>
       </c>
       <c r="D10" s="88"/>
@@ -3841,7 +3788,7 @@
         <v>35</v>
       </c>
       <c r="B15" s="90" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="E15" s="64"/>
     </row>
@@ -3932,7 +3879,9 @@
       <c r="A25" s="93" t="s">
         <v>191</v>
       </c>
-      <c r="B25" s="95"/>
+      <c r="B25" s="95">
+        <v>100</v>
+      </c>
       <c r="C25" s="80" t="s">
         <v>12</v>
       </c>
@@ -3957,7 +3906,13 @@
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{44517C17-9EE6-384B-9ACB-AD37EBBD9C0F}">
+          <x14:formula1>
+            <xm:f>'Dropdown Items'!$A$17:$A$20</xm:f>
+          </x14:formula1>
+          <xm:sqref>B5</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{ED4AF6AF-8563-A045-A93E-4862A40B6C70}">
           <x14:formula1>
             <xm:f>'Dropdown Items'!$B$17:$B$20</xm:f>
@@ -3998,8 +3953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A6BB566-6734-43D2-B721-97B73307DE8D}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4021,19 +3976,19 @@
       <c r="B1" s="41"/>
       <c r="C1" s="7"/>
       <c r="D1" s="7"/>
-      <c r="F1" s="112" t="s">
+      <c r="F1" s="110" t="s">
         <v>197</v>
       </c>
-      <c r="G1" s="113"/>
-      <c r="H1" s="113"/>
-      <c r="I1" s="114"/>
+      <c r="G1" s="111"/>
+      <c r="H1" s="111"/>
+      <c r="I1" s="112"/>
     </row>
     <row r="2" spans="1:9" ht="130.19999999999999" customHeight="1">
-      <c r="A2" s="110" t="s">
+      <c r="A2" s="108" t="s">
         <v>193</v>
       </c>
-      <c r="B2" s="111"/>
-      <c r="C2" s="111"/>
+      <c r="B2" s="109"/>
+      <c r="C2" s="109"/>
       <c r="D2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
@@ -4072,7 +4027,7 @@
       <c r="A5" s="55" t="s">
         <v>224</v>
       </c>
-      <c r="B5" s="54">
+      <c r="B5" s="90">
         <v>0</v>
       </c>
       <c r="C5" s="56" t="s">
@@ -4096,8 +4051,8 @@
       <c r="A6" s="55" t="s">
         <v>225</v>
       </c>
-      <c r="B6" s="54" t="s">
-        <v>394</v>
+      <c r="B6" s="90" t="s">
+        <v>387</v>
       </c>
       <c r="C6" s="56"/>
       <c r="D6" s="57"/>
@@ -4113,10 +4068,10 @@
       <c r="A7" s="55" t="s">
         <v>226</v>
       </c>
-      <c r="B7" s="54">
+      <c r="B7" s="90">
         <v>40</v>
       </c>
-      <c r="C7" s="44" t="s">
+      <c r="C7" s="56" t="s">
         <v>227</v>
       </c>
       <c r="D7" s="57"/>
@@ -4130,7 +4085,7 @@
       <c r="A8" s="55" t="s">
         <v>228</v>
       </c>
-      <c r="B8" s="18">
+      <c r="B8" s="90">
         <v>130</v>
       </c>
       <c r="C8" s="70" t="s">
@@ -4148,12 +4103,12 @@
       <c r="A9" s="50" t="s">
         <v>231</v>
       </c>
-      <c r="B9" s="105" t="s">
+      <c r="B9" s="30" t="s">
         <v>159</v>
       </c>
       <c r="C9" s="71"/>
       <c r="D9" s="72" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
       <c r="I9" s="4"/>
     </row>
@@ -4206,6 +4161,9 @@
       <c r="I15" s="4"/>
     </row>
     <row r="16" spans="1:9" ht="15.6">
+      <c r="A16" s="40"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
       <c r="F16" s="45" t="s">
         <v>205</v>
       </c>
@@ -4220,9 +4178,6 @@
       </c>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="40"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
       <c r="F17" s="55" t="s">
         <v>214</v>
       </c>
@@ -4405,12 +4360,18 @@
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{516E6F7D-20E1-4F3C-BB23-91F084FFA7DA}">
+          <x14:formula1>
+            <xm:f>'Dropdown Items'!$F$17:$F$20</xm:f>
+          </x14:formula1>
+          <xm:sqref>B13</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B33AC1E5-6F23-41DB-9A12-64441373EF4F}">
           <x14:formula1>
             <xm:f>'Dropdown Items'!$C$45:$C$49</xm:f>
           </x14:formula1>
-          <xm:sqref>G23 G36 G14 G29 B9</xm:sqref>
+          <xm:sqref>B9 G36 G14 G29 G23</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1FDF5500-C0F5-4891-9D07-E8EB27D70C01}">
           <x14:formula1>
@@ -4435,7 +4396,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
@@ -4747,8 +4708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E323FD3-6C48-44BB-9F06-8E13A7AFDEDD}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
@@ -4769,19 +4730,19 @@
       </c>
       <c r="B1" s="41"/>
       <c r="C1" s="7"/>
-      <c r="F1" s="112" t="s">
+      <c r="F1" s="110" t="s">
         <v>197</v>
       </c>
-      <c r="G1" s="113"/>
-      <c r="H1" s="113"/>
-      <c r="I1" s="114"/>
+      <c r="G1" s="111"/>
+      <c r="H1" s="111"/>
+      <c r="I1" s="112"/>
     </row>
     <row r="2" spans="1:9" ht="127.5" customHeight="1">
-      <c r="A2" s="110" t="s">
+      <c r="A2" s="108" t="s">
         <v>193</v>
       </c>
-      <c r="B2" s="111"/>
-      <c r="C2" s="111"/>
+      <c r="B2" s="109"/>
+      <c r="C2" s="109"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -5149,10 +5110,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74937810-402C-794A-86DB-3B61877792EA}">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="108" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
@@ -5172,10 +5133,10 @@
       <c r="C1" s="7"/>
     </row>
     <row r="2" spans="1:7" s="10" customFormat="1" ht="60" customHeight="1">
-      <c r="A2" s="115" t="s">
+      <c r="A2" s="113" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="115"/>
+      <c r="B2" s="113"/>
     </row>
     <row r="3" spans="1:7" ht="15" thickBot="1"/>
     <row r="4" spans="1:7" s="10" customFormat="1" ht="16.95" customHeight="1">
@@ -5205,7 +5166,9 @@
       <c r="A5" s="42" t="s">
         <v>271</v>
       </c>
-      <c r="B5" s="39"/>
+      <c r="B5" s="30" t="s">
+        <v>373</v>
+      </c>
       <c r="G5" s="64"/>
     </row>
     <row r="6" spans="1:7">
@@ -5232,7 +5195,7 @@
         <v>272</v>
       </c>
       <c r="B8" s="39" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
       <c r="G8" s="64"/>
     </row>
@@ -5254,7 +5217,9 @@
       <c r="A11" s="102" t="s">
         <v>275</v>
       </c>
-      <c r="B11" s="39"/>
+      <c r="B11" s="39">
+        <v>2.02E-4</v>
+      </c>
       <c r="C11" t="s">
         <v>100</v>
       </c>
@@ -5290,9 +5255,7 @@
       <c r="A14" s="102" t="s">
         <v>278</v>
       </c>
-      <c r="B14" s="39">
-        <v>2.02E-4</v>
-      </c>
+      <c r="B14" s="39"/>
       <c r="C14" t="s">
         <v>100</v>
       </c>
@@ -5371,31 +5334,28 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="42" t="s">
-        <v>281</v>
+        <v>376</v>
       </c>
-      <c r="B21" s="39">
-        <v>-3</v>
-      </c>
-      <c r="C21" t="s">
-        <v>98</v>
+      <c r="B21" s="31" t="s">
+        <v>379</v>
       </c>
       <c r="G21" s="64"/>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="42" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
-      <c r="B22" s="39"/>
+      <c r="B22" s="39">
+        <v>-3</v>
+      </c>
       <c r="C22" t="s">
         <v>98</v>
       </c>
-      <c r="G22" s="64" t="s">
-        <v>283</v>
-      </c>
+      <c r="G22" s="64"/>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="42" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B23" s="39"/>
       <c r="C23" t="s">
@@ -5407,7 +5367,7 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="42" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B24" s="39"/>
       <c r="C24" t="s">
@@ -5417,18 +5377,30 @@
         <v>283</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15" thickBot="1">
-      <c r="A25" s="50" t="s">
+    <row r="25" spans="1:7">
+      <c r="A25" s="42" t="s">
+        <v>285</v>
+      </c>
+      <c r="B25" s="39"/>
+      <c r="C25" t="s">
+        <v>98</v>
+      </c>
+      <c r="G25" s="64" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15" thickBot="1">
+      <c r="A26" s="50" t="s">
         <v>290</v>
       </c>
-      <c r="B25" s="86"/>
-      <c r="C25" s="80" t="s">
+      <c r="B26" s="86"/>
+      <c r="C26" s="80" t="s">
         <v>99</v>
       </c>
-      <c r="D25" s="31"/>
-      <c r="E25" s="86"/>
-      <c r="F25" s="80"/>
-      <c r="G25" s="82"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="86"/>
+      <c r="F26" s="80"/>
+      <c r="G26" s="82"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5437,7 +5409,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F576FF07-91DD-47FB-9E5A-B5DCBCB1E130}">
           <x14:formula1>
             <xm:f>'Dropdown Items'!$C$45:$C$49</xm:f>
@@ -5448,7 +5420,19 @@
           <x14:formula1>
             <xm:f>'Dropdown Items'!$B$55:$B$57</xm:f>
           </x14:formula1>
-          <xm:sqref>D11:D20 D25</xm:sqref>
+          <xm:sqref>D26 D11:D20</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{53FBF05B-62BD-4E4C-BFDB-E8E20678C5EF}">
+          <x14:formula1>
+            <xm:f>'Dropdown Items'!$C$55:$C$57</xm:f>
+          </x14:formula1>
+          <xm:sqref>B5</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7A804F1F-40D3-43ED-AAA3-2475022AB8DB}">
+          <x14:formula1>
+            <xm:f>'Dropdown Items'!$D$55:$D$56</xm:f>
+          </x14:formula1>
+          <xm:sqref>B21</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5460,8 +5444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60FD2D44-9B1B-421A-86D6-11D29F42E873}">
   <dimension ref="A1:XEX44"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="113" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
@@ -5493,11 +5477,11 @@
       <c r="F1" s="7"/>
     </row>
     <row r="2" spans="1:1018 1026:2042 2050:3066 3074:4090 4098:5114 5122:6138 6146:7162 7170:8186 8194:9210 9218:10234 10242:11258 11266:12282 12290:13306 13314:14330 14338:15354 15362:16378" s="10" customFormat="1" ht="60" customHeight="1">
-      <c r="A2" s="115" t="s">
+      <c r="A2" s="113" t="s">
         <v>88</v>
       </c>
-      <c r="B2" s="115"/>
-      <c r="C2" s="115"/>
+      <c r="B2" s="113"/>
+      <c r="C2" s="113"/>
       <c r="D2" s="19"/>
       <c r="E2" s="19"/>
     </row>
@@ -7581,7 +7565,7 @@
         <v>317</v>
       </c>
       <c r="B5" s="39" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
       <c r="C5"/>
       <c r="D5"/>
@@ -7644,7 +7628,7 @@
         <v>318</v>
       </c>
       <c r="B12" s="39" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
       <c r="C12"/>
       <c r="D12"/>
@@ -7703,7 +7687,7 @@
         <v>304</v>
       </c>
       <c r="B19" s="39" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="C19"/>
       <c r="D19"/>
@@ -7794,7 +7778,7 @@
         <v>316</v>
       </c>
       <c r="B28" s="39" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
       <c r="C28"/>
       <c r="D28"/>
@@ -7805,7 +7789,9 @@
       <c r="A29" s="42" t="s">
         <v>311</v>
       </c>
-      <c r="B29" s="39"/>
+      <c r="B29" s="39">
+        <v>17.600000000000001</v>
+      </c>
       <c r="C29" t="s">
         <v>315</v>
       </c>
@@ -7820,9 +7806,7 @@
       <c r="B30" s="39">
         <v>75</v>
       </c>
-      <c r="C30" t="s">
-        <v>315</v>
-      </c>
+      <c r="C30"/>
       <c r="D30" s="31"/>
       <c r="E30" s="39"/>
       <c r="F30" s="43"/>
@@ -7853,9 +7837,7 @@
       <c r="A33" s="42" t="s">
         <v>312</v>
       </c>
-      <c r="B33" s="39">
-        <v>17.600000000000001</v>
-      </c>
+      <c r="B33" s="39"/>
       <c r="C33" t="s">
         <v>315</v>
       </c>
@@ -7986,7 +7968,7 @@
   <dimension ref="A1:XEY101"/>
   <sheetViews>
     <sheetView zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
@@ -8005,10 +7987,10 @@
       <c r="B1" s="6"/>
     </row>
     <row r="2" spans="1:4" s="10" customFormat="1" ht="36" customHeight="1">
-      <c r="A2" s="115" t="s">
+      <c r="A2" s="113" t="s">
         <v>365</v>
       </c>
-      <c r="B2" s="115"/>
+      <c r="B2" s="113"/>
     </row>
     <row r="3" spans="1:4" s="10" customFormat="1" ht="16.95" customHeight="1" thickBot="1">
       <c r="A3" s="19"/>

</xml_diff>